<commit_message>
feat: Implement a new timber reporting module, including quantity tracking for mutation records and various report templates.
</commit_message>
<xml_diff>
--- a/public/template/laporan/Laporan Mutasi Kayu Bulat.xlsx
+++ b/public/template/laporan/Laporan Mutasi Kayu Bulat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\PKL\PKL_DLH_uji2\public\template\laporan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D348F69F-C122-40F4-9380-AFE219C03B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0499EE82-0798-4732-8942-6602248FF773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{2AD5A86D-9142-4266-931F-E0186FCDEF72}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AD5A86D-9142-4266-931F-E0186FCDEF72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>Bulan / Tahun</t>
   </si>
@@ -109,17 +109,29 @@
     <t>50.12</t>
   </si>
   <si>
-    <t>2,789.71</t>
-  </si>
-  <si>
     <t>* Jangan Ubah Format Excel</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Jumlah Btg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +176,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -197,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -291,11 +309,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -312,47 +356,80 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="14">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -362,6 +439,18 @@
           <color indexed="64"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -911,32 +1000,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01782300-FA2E-4D87-80D0-1A82FA14221C}" name="Table1" displayName="Table1" ref="A15:G25" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A15:G25" xr:uid="{01782300-FA2E-4D87-80D0-1A82FA14221C}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01782300-FA2E-4D87-80D0-1A82FA14221C}" name="Table1" displayName="Table1" ref="A15:K25" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A15:K25" xr:uid="{01782300-FA2E-4D87-80D0-1A82FA14221C}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{78221867-DB57-4FA1-B9A2-466F865756F7}" name="1"/>
     <tableColumn id="2" xr3:uid="{368BDB1D-2724-4AA5-935B-DF89458B0CB1}" name="2"/>
     <tableColumn id="3" xr3:uid="{D78980AA-1F45-4E9C-B10B-2AC5E08AA869}" name="3"/>
-    <tableColumn id="4" xr3:uid="{F5F22384-7163-4844-8016-D921DB394424}" name="4" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{F5F22384-7163-4844-8016-D921DB394424}" name="4" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{6E3A490B-E5DE-4D99-BAEB-2BC0E0DE8F18}" name="5"/>
     <tableColumn id="6" xr3:uid="{B935BDF1-4E07-4EDC-9CC8-1934ACB8B730}" name="6"/>
     <tableColumn id="7" xr3:uid="{B7608A8C-2CAE-4DFE-828C-5AEE13837FCE}" name="7"/>
+    <tableColumn id="8" xr3:uid="{E2E90749-5509-4441-8A5E-96368C095C2A}" name="8" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{C6E4168B-AFC9-426B-AF1B-9F5EAB2511B6}" name="9" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{DA13DA0B-B27C-4987-BA3F-5DF9E79A217F}" name="10" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{B3B060C1-BC5F-4479-B927-1280A1BF35CD}" name="11" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{09BAC9DB-FD97-44C2-899D-6D848CA80A49}" name="Table13" displayName="Table13" ref="A15:G25" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A15:G25" xr:uid="{09BAC9DB-FD97-44C2-899D-6D848CA80A49}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{09D3504C-94B3-48BA-A9F4-B813A1BE2E99}" name="1"/>
-    <tableColumn id="2" xr3:uid="{1FBEA9DE-492E-405F-8F3C-BABC2D0F35A2}" name="2"/>
-    <tableColumn id="3" xr3:uid="{33CB0466-388D-41DC-8989-3FE200E3EC4E}" name="3"/>
-    <tableColumn id="4" xr3:uid="{636BC61C-7CE3-4C7E-9ED4-2C26ACEE7A0C}" name="4" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{9AE7EF3C-A2A3-4BF7-9269-D552ACF0AE21}" name="5"/>
-    <tableColumn id="6" xr3:uid="{D191D9EA-ABBE-468D-95D4-4A5DFA01D011}" name="6"/>
-    <tableColumn id="7" xr3:uid="{73F44B9F-1B46-4B05-B433-532C369D4F71}" name="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CCF8B109-4196-401B-8510-6DE44E79C71C}" name="Table15" displayName="Table15" ref="A15:K25" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A15:K25" xr:uid="{CCF8B109-4196-401B-8510-6DE44E79C71C}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{E1053F37-F035-4703-8926-61F111133223}" name="1"/>
+    <tableColumn id="2" xr3:uid="{CDCC01B1-5460-42CE-B931-B9544D846F5C}" name="2"/>
+    <tableColumn id="3" xr3:uid="{43E95DF0-E282-41CB-A2BA-3A61DB2083CC}" name="3"/>
+    <tableColumn id="4" xr3:uid="{EC3202A2-F672-4762-A91F-A089687EB73A}" name="4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{FB6D7716-B8DB-463D-9826-E38CA6088F5A}" name="5"/>
+    <tableColumn id="6" xr3:uid="{9571215B-E13A-437F-93A3-BEF7A10021CE}" name="6"/>
+    <tableColumn id="7" xr3:uid="{AB5BE11C-AF40-4BBB-AC59-8F190F05A38C}" name="7"/>
+    <tableColumn id="8" xr3:uid="{DAF988F0-841C-412A-9CC9-70767C59D24F}" name="8" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{CE8DDD1B-44CF-419C-BB1F-7285CD0FC2F6}" name="9" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{83131B58-C112-4F82-B678-783BD5D72FE3}" name="10" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{B654B710-DE35-4369-AA39-CB3FE957FC14}" name="11" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1239,25 +1336,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC405B0-C0B1-40C5-8B45-93D30DF96482}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.81640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.90625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.08984375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="21.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.453125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.90625" style="2"/>
+    <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="17" t="s">
@@ -1268,7 +1369,7 @@
       <c r="F1" s="4"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="17" t="s">
@@ -1278,7 +1379,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="17" t="s">
@@ -1288,15 +1389,15 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1304,7 +1405,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1312,7 +1413,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1320,7 +1421,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1328,7 +1429,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1336,7 +1437,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1344,7 +1445,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="5"/>
       <c r="C11" s="1"/>
@@ -1352,57 +1453,73 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="15" t="s">
-        <v>25</v>
+      <c r="B12" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="21"/>
+      <c r="G13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="H13" s="19"/>
+      <c r="I13" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="J13" s="19"/>
+      <c r="K13" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>8</v>
+      <c r="E14" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1424,8 +1541,20 @@
       <c r="G15" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -1433,7 +1562,7 @@
       <c r="F16"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -1441,7 +1570,7 @@
       <c r="F17"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -1449,7 +1578,7 @@
       <c r="F18"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -1457,7 +1586,7 @@
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -1465,7 +1594,7 @@
       <c r="F20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -1473,7 +1602,7 @@
       <c r="F21"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -1481,7 +1610,7 @@
       <c r="F22"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -1489,7 +1618,7 @@
       <c r="F23"/>
       <c r="G23"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -1497,7 +1626,7 @@
       <c r="F24"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -1506,13 +1635,18 @@
       <c r="G25"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1524,25 +1658,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37EB156-6D6C-48BA-8F3F-7F35DFE6AEDC}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A3" zoomScale="94" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="C4" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.81640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.90625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.08984375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="21.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.453125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.90625" style="2"/>
+    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.21875" style="2" customWidth="1"/>
+    <col min="9" max="10" width="19.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="17" t="s">
@@ -1553,7 +1688,7 @@
       <c r="F1" s="4"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="17" t="s">
@@ -1563,7 +1698,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="17" t="s">
@@ -1573,15 +1708,15 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1589,7 +1724,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1597,7 +1732,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1605,7 +1740,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1613,7 +1748,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1621,7 +1756,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1629,7 +1764,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1637,57 +1772,73 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="15" t="s">
-        <v>25</v>
+      <c r="B12" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="21"/>
+      <c r="G13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="H13" s="19"/>
+      <c r="I13" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="J13" s="19"/>
+      <c r="K13" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>8</v>
+      <c r="E14" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1709,50 +1860,60 @@
       <c r="G15" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="10">
+      <c r="H15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="11">
         <v>1</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="10">
+      <c r="D16" s="15">
+        <v>2789.71</v>
+      </c>
+      <c r="F16" s="11">
         <v>0</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="H16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="J16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G16"/>
-    </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="11">
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12">
         <v>2</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="14">
+      <c r="D17" s="16">
         <v>0</v>
       </c>
-      <c r="D17" s="14">
+      <c r="F17" s="13">
         <v>0</v>
       </c>
-      <c r="E17" s="14">
+      <c r="H17" s="16">
         <v>0</v>
       </c>
-      <c r="F17" s="14">
+      <c r="J17" s="13">
         <v>0</v>
       </c>
-      <c r="G17"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -1760,7 +1921,7 @@
       <c r="F18"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -1768,7 +1929,7 @@
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -1776,7 +1937,7 @@
       <c r="F20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -1784,7 +1945,7 @@
       <c r="F21"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -1792,7 +1953,7 @@
       <c r="F22"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -1800,7 +1961,7 @@
       <c r="F23"/>
       <c r="G23"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -1808,7 +1969,7 @@
       <c r="F24"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -1817,12 +1978,16 @@
       <c r="G25"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="I13:J13"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>